<commit_message>
added Docs files a bit
</commit_message>
<xml_diff>
--- a/Taxonomy - LLMS.xlsx
+++ b/Taxonomy - LLMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Banwa\Documents\RESEARCH WORK AND PATENTS\WORKING PAPERS\GITHUB REPOSITORIES\LLM-Evolution-Metadata-Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E0D1D5-35A6-4FAE-9C00-BFCB3F1226FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932DD011-3FB8-4486-B202-31A839BDA7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C2ABDBC-78BC-4B8E-BC0A-2D64AD85A683}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="181">
   <si>
     <t>Architecture Family</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Context Learning</t>
   </si>
   <si>
-    <t>BERT</t>
-  </si>
-  <si>
     <t>Encoder-Only</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>RoBERTa</t>
-  </si>
-  <si>
     <t>160 GB Text</t>
   </si>
   <si>
@@ -574,6 +568,15 @@
   </si>
   <si>
     <t>Grok 4 (xAI),2025</t>
+  </si>
+  <si>
+    <t>BERT(Large)</t>
+  </si>
+  <si>
+    <t>RoBERTa(Large)</t>
+  </si>
+  <si>
+    <t>355 M</t>
   </si>
 </sst>
 </file>
@@ -964,13 +967,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB46CDC-1974-4808-8FD6-CB4DA1B870FD}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.21875" customWidth="1"/>
@@ -1026,16 +1029,16 @@
     </row>
     <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="B2" s="1">
         <v>2018</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -1047,16 +1050,16 @@
         <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
@@ -1065,76 +1068,76 @@
     </row>
     <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>179</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>180</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>15</v>
@@ -1143,7 +1146,7 @@
     </row>
     <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1">
         <v>2020</v>
@@ -1152,67 +1155,67 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1">
         <v>2022</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>17</v>
@@ -1221,230 +1224,230 @@
     </row>
     <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1">
         <v>2022</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1">
         <v>2022</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1">
         <v>2021</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" s="1">
         <v>2021</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" s="1">
         <v>2022</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1">
         <v>2023</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>18</v>
@@ -1452,209 +1455,209 @@
     </row>
     <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1">
         <v>2023</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B14" s="1">
         <v>2022</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B15" s="1">
         <v>2022</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="I15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="1">
         <v>2022</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="K16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B17" s="1">
         <v>2021</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B18" s="1">
         <v>2023</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>25</v>
@@ -1669,10 +1672,10 @@
         <v>23</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>27</v>
@@ -1680,19 +1683,19 @@
     </row>
     <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B19" s="1">
         <v>2024</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>25</v>
@@ -1701,24 +1704,24 @@
         <v>23</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B20" s="1">
         <v>2024</v>
@@ -1727,10 +1730,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
@@ -1745,10 +1748,10 @@
         <v>23</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>24</v>
@@ -1756,268 +1759,268 @@
     </row>
     <row r="21" spans="1:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B21" s="1">
         <v>2024</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="I21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B22" s="1">
         <v>2024</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="I22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="K22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B23" s="1">
         <v>2025</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="K23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B24" s="3">
         <v>2025</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B25" s="3">
         <v>2025</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B26" s="3">
         <v>2025</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B27" s="3">
         <v>2025</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2032,6 +2035,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B00AE45020F33547B7F780CDDCD41EC8" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="966c3ad6a514153134e2633815ac4996">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3f047075-99eb-4061-85c8-a5cb9b0e18af" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e892cf9307a3f76ccdc7fbfbda7c4d5d" ns3:_="">
     <xsd:import namespace="3f047075-99eb-4061-85c8-a5cb9b0e18af"/>
@@ -2175,15 +2187,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2191,6 +2194,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{656861FE-66B5-4A15-8568-895DB459A815}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{624A0F0D-064D-43C4-BA9A-259EC1F61D39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2204,14 +2215,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{656861FE-66B5-4A15-8568-895DB459A815}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>